<commit_message>
Successfully created batter-pitcher interaction
</commit_message>
<xml_diff>
--- a/HOUWAS stats.xlsx
+++ b/HOUWAS stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\HackReactor\MVP-baseball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826BCF21-DDFF-4525-9873-A08AC8255382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E277656-EE85-48C6-8AF8-5BCD1973BD6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4233F5CA-3CC5-438D-B92B-855C505FCEE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4233F5CA-3CC5-438D-B92B-855C505FCEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DA60D6-871C-4562-9EE9-A1FFAB5DABF2}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C81585-97A2-49A7-B6D6-C3C4EF08B56C}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,6 +1623,27 @@
       <c r="B35">
         <v>4</v>
       </c>
+      <c r="D35">
+        <f>993/4083</f>
+        <v>0.24320352681851579</v>
+      </c>
+      <c r="E35">
+        <f>346/4083</f>
+        <v>8.4741611560127356E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.83</v>
+      </c>
+      <c r="G35">
+        <v>0.122</v>
+      </c>
+      <c r="H35">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="I35">
+        <f>254/975</f>
+        <v>0.26051282051282049</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Properly looping through lineup for WAS, even if not keeping track of individual batter results
</commit_message>
<xml_diff>
--- a/HOUWAS stats.xlsx
+++ b/HOUWAS stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\HackReactor\MVP-baseball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E277656-EE85-48C6-8AF8-5BCD1973BD6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080BBE64-8E18-4179-BB40-0FDDE8E999C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4233F5CA-3CC5-438D-B92B-855C505FCEE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4233F5CA-3CC5-438D-B92B-855C505FCEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DA60D6-871C-4562-9EE9-A1FFAB5DABF2}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C81585-97A2-49A7-B6D6-C3C4EF08B56C}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Built out list of potential results for runners on walk and single
</commit_message>
<xml_diff>
--- a/HOUWAS stats.xlsx
+++ b/HOUWAS stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\HackReactor\MVP-baseball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080BBE64-8E18-4179-BB40-0FDDE8E999C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D26B143-B8CD-43D1-8D74-971C4010CCA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4233F5CA-3CC5-438D-B92B-855C505FCEE5}"/>
   </bookViews>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C81585-97A2-49A7-B6D6-C3C4EF08B56C}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1496,7 +1496,7 @@
         <v>0.99</v>
       </c>
       <c r="G28">
-        <v>1.01</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="H28">
         <v>0.29499999999999998</v>

</xml_diff>